<commit_message>
Used constants in test files
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -162,24 +162,6 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -244,6 +226,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -258,12 +256,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -280,12 +280,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C5"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Username" dataDxfId="3"/>
-    <tableColumn id="2" name="Password" dataDxfId="2"/>
-    <tableColumn id="3" name="Expected Result" dataDxfId="1"/>
+    <tableColumn id="1" name="Username" dataDxfId="2"/>
+    <tableColumn id="2" name="Password" dataDxfId="1"/>
+    <tableColumn id="3" name="Expected Result" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -557,7 +557,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>